<commit_message>
Se agregó el plot de porcentaje automatizado para todas o para algunas cepas/condiciones
</commit_message>
<xml_diff>
--- a/files/proteome_Schmidt/Proteome_size.xlsx
+++ b/files/proteome_Schmidt/Proteome_size.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eli\Documents\🦄Maestria_coronavirus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elisamarquez/Documents/UtrillaLab/Publicacion/files/proteome_Schmidt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27569DDE-4648-4EC5-809A-17CC59F8B6A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104278ED-2935-4542-A132-E8ADB2AD627F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20740" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>Glicerol</t>
   </si>
   <si>
-    <t>Piruvate</t>
-  </si>
-  <si>
     <t>Quimiostato µ=0.5</t>
   </si>
   <si>
@@ -81,12 +78,6 @@
     <t>pH6 glucosa</t>
   </si>
   <si>
-    <t>Xylosa</t>
-  </si>
-  <si>
-    <t>Mannosa</t>
-  </si>
-  <si>
     <t>Galactosa</t>
   </si>
   <si>
@@ -94,6 +85,15 @@
   </si>
   <si>
     <t>Fructosa</t>
+  </si>
+  <si>
+    <t>Piruvato</t>
+  </si>
+  <si>
+    <t>Xilosa</t>
+  </si>
+  <si>
+    <t>Manosa</t>
   </si>
 </sst>
 </file>
@@ -423,12 +423,12 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:W1"/>
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -451,52 +451,52 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>

</xml_diff>